<commit_message>
checks for stable eigenvalues of matrix A done
</commit_message>
<xml_diff>
--- a/PCAcombined/PCAcombined_predicted_factors_matrix_10.xlsx
+++ b/PCAcombined/PCAcombined_predicted_factors_matrix_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,132 @@
       <c r="E1" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -466,6 +592,132 @@
       <c r="E2" t="n">
         <v>0.1715341279625983</v>
       </c>
+      <c r="F2" t="n">
+        <v>0.1457595503430866</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1184938692095354</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.09065835301098701</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.06276232661485803</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.03510674917016914</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.007873310382443755</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.01882964164635714</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.04494033554773513</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-0.07042682863953015</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-0.09527617472591725</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-0.1194873423249048</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-0.1430665907925116</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-0.1660244758469021</v>
+      </c>
+      <c r="S2" t="n">
+        <v>-0.188373935378442</v>
+      </c>
+      <c r="T2" t="n">
+        <v>-0.2101290872844682</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-0.2313044921692987</v>
+      </c>
+      <c r="V2" t="n">
+        <v>-0.2519147158124612</v>
+      </c>
+      <c r="W2" t="n">
+        <v>-0.2719740819697067</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-0.2914965436670746</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>-0.3104956263712677</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>-0.3289844132040425</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>-0.3469755534336151</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>-0.3644812826934565</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-0.3815134480281674</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>-0.3980835338163325</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>-0.4142026864572875</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>-0.4298817368244769</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>-0.4451312201428768</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>-0.4599613933126349</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>-0.4743822498873194</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>-0.4884035329945663</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>-0.5020347465048829</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>-0.5152851647393545</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>-0.5281638409762243</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>-0.5406796149796953</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>-0.5528411197378843</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>-0.5646567875631905</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>-0.576134855678868</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>-0.587283371390718</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>-0.5981101969220954</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>-0.6086230139737091</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>-0.6188293280561653</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -483,6 +735,132 @@
       <c r="E3" t="n">
         <v>0.05749480467915952</v>
       </c>
+      <c r="F3" t="n">
+        <v>0.04120347659622019</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.03107684447476144</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.02520330481767082</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.02225111644283355</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.02130054821895204</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.02171690581688993</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.02306132438921547</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.02502951965954952</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.02740996219418383</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.0300552836151321</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.03286266128805421</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.03576030701061099</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.03869812215776639</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.04164120969825835</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.04456535384593253</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.04745386049793014</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.05029534231704061</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.05308216182022265</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.05580933424380467</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.05847375259901872</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.06107363910812076</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.06360815610154548</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.06607712950457646</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.06848085199798234</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.07081994268050951</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.07309524688200641</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.07530776456317484</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.07745859910593982</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.07954892067356772</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.08157993999827286</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.08355288964300603</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.0854690106280024</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0.08732954291278057</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.08913571865191729</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.0908887574481972</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.09258986304502272</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.09424022105637304</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.0958409974447864</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0.09739333753849215</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0.09889836543681892</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.1003571836948521</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.101770873208455</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -500,6 +878,132 @@
       <c r="E4" t="n">
         <v>-0.2170132521748957</v>
       </c>
+      <c r="F4" t="n">
+        <v>-0.1465926983597901</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.09839544594532712</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0.06547716579790441</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.04303063130960753</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.02775222688724133</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-0.01737774909621532</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.01035695745646588</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-0.005628879650026423</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-0.002467534361724918</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.0003762189873174977</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.0009848687054482522</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.001848169763094513</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.00237266577150194</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.002667077337524987</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.0028057377828558</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.002839454539551368</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.002802940822757317</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.002719900521797064</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.002606507315981235</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.002473785041139396</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.002329236235170534</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.002177956249288311</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.002023395361111431</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.00186788004176978</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.001712969437690387</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0.001559699114890173</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.001408747681442419</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.001260550658563702</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.001115378275340048</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.0009733885956257219</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.0008346637817745273</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.0006992348335869668</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.0005670984534374356</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.0004382285338391716</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0.0003125839739583174</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.0001901139912159509</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>7.076172468490228e-05</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>-4.553332565025128e-05</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>-0.0001588336523940957</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>-0.0002692026336164062</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>-0.0003767037923179358</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>-0.0004814003047574394</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -517,6 +1021,132 @@
       <c r="E5" t="n">
         <v>0.09645348336170805</v>
       </c>
+      <c r="F5" t="n">
+        <v>0.0674641094192273</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0476981886313939</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.03405493819575531</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0245328433869667</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.01780722021712111</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.01298884045013631</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.009475937313913045</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.006859363053943916</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.004860166127058434</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.003287849204986698</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.002012191474275804</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.0009441193008289815</v>
+      </c>
+      <c r="R5" t="n">
+        <v>2.267512742477385e-05</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-0.0007938777323262625</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-0.00153413436011389</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-0.002217705637078993</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-0.002858062064601421</v>
+      </c>
+      <c r="W5" t="n">
+        <v>-0.003464478997135344</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-0.004043366915402838</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>-0.004599180794598425</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>-0.005135041417924912</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>-0.005653159609958953</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-0.006155125689788559</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>-0.006642106800409534</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>-0.00711498131184944</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>-0.007574430274275648</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>-0.008020999580893496</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>-0.008455142175150662</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>-0.008877246676293409</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>-0.009287656772145721</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>-0.009686684343426779</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>-0.0100746183381378</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>-0.01045173076889142</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>-0.01081828076580722</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>-0.01117451731758497</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>-0.01152068112928473</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>-0.0118570058865281</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>-0.01218371912171151</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>-0.01250104281393364</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>-0.01280919381118136</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>-0.01310838413409908</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>-0.01339882120105376</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -534,6 +1164,132 @@
       <c r="E6" t="n">
         <v>-0.05998292198792372</v>
       </c>
+      <c r="F6" t="n">
+        <v>-0.03919722453945654</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-0.02550840725056183</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-0.01632136675455672</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-0.01011369621108868</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-0.00591430441114256</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-0.003079256377982191</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.001174278804646911</v>
+      </c>
+      <c r="M6" t="n">
+        <v>9.569901450742335e-05</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.0009318779531280711</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.001471711864697291</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.00180921320382429</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.002008732710854672</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.002114342636906199</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.002156239038205889</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.002155115968111229</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.00212515696024081</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.002076082478163395</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.002014552151318189</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.001945125658769542</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.001870921499351897</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.001794068835716978</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.001716017534385462</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.001637750983443339</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.001559932224962884</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.001483004329547724</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.001407259361285811</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0.00133288577468053</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0.001260000996561023</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.001188673828386184</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0.001118939851873226</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.001050812024282886</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.0009842879655712791</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.0009193549699300798</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.0008559934515653891</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.0007941793129188355</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.0007338855711460713</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.0006750834739466479</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.0006177432637932512</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.0005618347000477543</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0.0005073274143763233</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.0004541911513908303</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.000402395930291766</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -551,6 +1307,132 @@
       <c r="E7" t="n">
         <v>0.04058629798219291</v>
       </c>
+      <c r="F7" t="n">
+        <v>0.02736716800441029</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.01830182419749269</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.01213923934922288</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.007974789760905864</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.005177452952313205</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.003312996061292551</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.002084219209986745</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.001288148646236076</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0007862730625554588</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.0004840948819388538</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.0003171495241136208</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.0002414642447088328</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.0002270499443077536</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.0002534615057646363</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.0003067684100238668</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.0003774870553997271</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.0004591691476852126</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.0005474378430852863</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.0006393295774798718</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.0007328446444979862</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.0008266403476297706</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.0009198215358122393</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.001011797654294622</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.001102185222603147</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.001190741331965664</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.001277318318977655</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.001361832891324409</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0.001444245112813016</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0.001524544111501242</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0.001602738369934568</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0.001678849136429838</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0.001752905960752306</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0.001824943674667143</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0.001895000354293776</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0.00196311594895199</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0.002029331361884516</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0.002093687836955282</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.002156226552198515</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0.002216988352943676</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0.002276013578930048</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.002333341954530729</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.002389012521243727</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -568,6 +1450,132 @@
       <c r="E8" t="n">
         <v>0.004784864384435281</v>
       </c>
+      <c r="F8" t="n">
+        <v>0.002815002841379589</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.001596163845163658</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0008389756281939909</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.000358065402516711</v>
+      </c>
+      <c r="J8" t="n">
+        <v>4.367022587927413e-05</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-0.0001685256076303651</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-0.0003167372646968563</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-0.0004241595413071084</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-0.0005051698832355654</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-0.0005688404633573234</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-0.0006209758005427264</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-0.0006653278321946488</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-0.0007043392237024305</v>
+      </c>
+      <c r="S8" t="n">
+        <v>-0.0007396079830000132</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-0.0007721828761757353</v>
+      </c>
+      <c r="U8" t="n">
+        <v>-0.0008027537027287713</v>
+      </c>
+      <c r="V8" t="n">
+        <v>-0.0008317749991959619</v>
+      </c>
+      <c r="W8" t="n">
+        <v>-0.0008595469753831973</v>
+      </c>
+      <c r="X8" t="n">
+        <v>-0.0008862686771119334</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>-0.0009120729731248023</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>-0.0009370495856579662</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>-0.0009612602318185689</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>-0.000984748552429597</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>-0.001007546597313749</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>-0.001029679038887892</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>-0.001051165891081551</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>-0.001072024248562114</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>-0.001092269387073512</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>-0.001111915449836837</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>-0.001130975867950142</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>-0.001149463611616277</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>-0.001167391335207493</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>-0.001184771456828151</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>-0.001201616198419998</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>-0.001217937602846407</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>-0.001233747538200436</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>-0.001249057695588409</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>-0.001263879584096807</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>-0.001278224525048892</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>-0.001292103646688867</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>-0.001305527879824337</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>-0.001318507954617133</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -585,6 +1593,132 @@
       <c r="E9" t="n">
         <v>0.02304804663316733</v>
       </c>
+      <c r="F9" t="n">
+        <v>0.01345771107617472</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.007348571115719802</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.003384255331990467</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0007950517842490522</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-0.000892022591241066</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-0.001979606717141797</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-0.002666060299183203</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-0.00308323759239518</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-0.003319510376981851</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-0.003434395573862704</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-0.003468090750598504</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-0.00344778806140126</v>
+      </c>
+      <c r="R9" t="n">
+        <v>-0.00339189515760436</v>
+      </c>
+      <c r="S9" t="n">
+        <v>-0.003312873707470632</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-0.003219155483761544</v>
+      </c>
+      <c r="U9" t="n">
+        <v>-0.003116438932531713</v>
+      </c>
+      <c r="V9" t="n">
+        <v>-0.00300856791521507</v>
+      </c>
+      <c r="W9" t="n">
+        <v>-0.002898127872228042</v>
+      </c>
+      <c r="X9" t="n">
+        <v>-0.002786850524249217</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>-0.002675888687842924</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>-0.002566002907833248</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>-0.002457688190292332</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>-0.002351260038101898</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>-0.002246912833794418</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>-0.002144759434987305</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>-0.002044858008534375</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>-0.00194723019975513</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>-0.001851873421002752</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>-0.001758769151600345</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>-0.0016678885344173</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>-0.001579196141804003</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>-0.001492652503127614</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>-0.001408215795576915</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>-0.001325842970400623</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>-0.001245490498867466</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>-0.001167114862568589</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>-0.0010906728722462</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>-0.001016121871939392</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>-0.0009434198666814325</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>-0.0008725255994654075</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>-0.000803398594704006</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>-0.0007359991797336377</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -602,6 +1736,132 @@
       <c r="E10" t="n">
         <v>0.005020559573845449</v>
       </c>
+      <c r="F10" t="n">
+        <v>0.003812125449567814</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.002714429953594295</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.001883086950180579</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.001305431480060944</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.000927597491306922</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0006958319988315028</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.0005670658783466444</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0005094832392549742</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.0005004339751498967</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.0005240876525282821</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.0005694872441612116</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0006290899216797477</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.0006977204805571701</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.0007718368225063288</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.0008490201799120379</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.0009276233926211678</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.001006528978213451</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.001084982975271212</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.0011624808993712</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.001238689475846276</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.001313392914572826</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0.001386456016319872</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.001457798824271581</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.001527379197602521</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.001595180823870622</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.0016612049677335</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0.001725464788231367</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>0.001787981423179296</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>0.001848781290243951</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>0.001907894226411969</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0.001965352205629953</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>0.00202118845550235</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>0.002075436849627076</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>0.002128131490462874</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>0.002179306424000437</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>0.002228995445643009</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>0.002277231969265005</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0.002324048940011569</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>0.00236947877740555</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>0.002413553339442275</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0.002456303901199562</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.002497761143478607</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -618,6 +1878,132 @@
       </c>
       <c r="E11" t="n">
         <v>-0.000599763343974584</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.0003670660207578433</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.0003495617047091887</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.0003615545015109313</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-0.0003636503029408758</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-0.0003519765091116753</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-0.0003298036673804032</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-0.0003007996427410805</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-0.0002677544357513555</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-0.0002325760023745555</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-0.0001965094295982725</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-0.0001603419864339391</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-0.000124555817532954</v>
+      </c>
+      <c r="R11" t="n">
+        <v>-8.94340317499334e-05</v>
+      </c>
+      <c r="S11" t="n">
+        <v>-5.513229926460575e-05</v>
+      </c>
+      <c r="T11" t="n">
+        <v>-2.172635941777675e-05</v>
+      </c>
+      <c r="U11" t="n">
+        <v>1.075689104692044e-05</v>
+      </c>
+      <c r="V11" t="n">
+        <v>4.23193453164732e-05</v>
+      </c>
+      <c r="W11" t="n">
+        <v>7.297896795498669e-05</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.0001027618963938967</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.0001316976712022902</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.000159816467860087</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0.0001871475860278826</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.000213718710647427</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.0002395556319394633</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.0002646822257877015</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.0002891205710652576</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0.0003128911291396084</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>0.0003360129419172315</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>0.000358503824367037</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>0.0003803805394857898</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0.000401658950852946</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>0.0004223541520186196</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>0.0004424805741429361</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>0.000462052074331636</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>0.0004810820074313923</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>0.0004995832840112686</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>0.0005175684170194141</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0.0005350495592827366</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>0.0005520385336725621</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>0.000568546857466309</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.0005845857621240901</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.0006001662094763168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>